<commit_message>
Created the interpolation function and cleaned up class code
</commit_message>
<xml_diff>
--- a/Assignment1.xlsx
+++ b/Assignment1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickleenders/Documents/GitHub/WTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F079089-10CC-5B40-B314-E85B84959835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0F23CA-FC13-A246-BDA8-74CF0F5264E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16460" xr2:uid="{D1415A2E-7014-BD45-803A-CAF9DE7FAA8F}"/>
   </bookViews>
@@ -25,18 +25,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>t/c</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="15"/>
@@ -66,10 +85,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -384,263 +404,277 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C15760-0CCB-7A46-9003-94C8709B67DB}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
+    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>2.8</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B2" s="2">
         <v>5.38</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C2" s="2">
         <v>14.5</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D2" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>11</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="2">
         <v>5.45</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="2">
         <v>14.43</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="2">
         <v>86.05</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>16.87</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="2">
         <v>5.87</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="2">
         <v>12.55</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="2">
         <v>61.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="5" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>22.96</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="2">
         <v>6.18</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="2">
         <v>8.89</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="2">
         <v>43.04</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="6" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>32.31</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="2">
         <v>6.02</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="2">
         <v>6.38</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="2">
         <v>32.42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>41.57</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="2">
         <v>5.42</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="2">
         <v>4.67</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="2">
         <v>27.81</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>50.41</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="2">
         <v>4.7</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="2">
         <v>2.89</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="2">
         <v>25.32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="9" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>58.53</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="2">
         <v>1.21</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="2">
         <v>24.26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="10" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>65.75</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="2">
         <v>3.4</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="2">
         <v>-0.13</v>
       </c>
-      <c r="D9" s="1">
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="D10" s="2">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>71.97</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="2">
         <v>2.91</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="2">
         <v>-1.1100000000000001</v>
       </c>
-      <c r="D10" s="1">
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="D11" s="2">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>77.19</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="2">
         <v>2.54</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="2">
         <v>-1.86</v>
       </c>
-      <c r="D11" s="1">
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="D12" s="2">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>78.709999999999994</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="2">
         <v>2.4300000000000002</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="2">
         <v>-2.08</v>
       </c>
-      <c r="D12" s="1">
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="D13" s="2">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>80.14</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="2">
         <v>2.33</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="2">
         <v>-2.2799999999999998</v>
       </c>
-      <c r="D13" s="1">
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="D14" s="2">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>82.71</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="2">
         <v>2.13</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C15" s="2">
         <v>-2.64</v>
       </c>
-      <c r="D14" s="1">
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="D15" s="2">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>84.93</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="2">
         <v>1.9</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="2">
         <v>-2.95</v>
       </c>
-      <c r="D15" s="1">
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="D16" s="2">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>86.83</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="2">
         <v>1.63</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C17" s="2">
         <v>-3.18</v>
       </c>
-      <c r="D16" s="1">
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="D17" s="2">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>88.45</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="2">
         <v>1.18</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="2">
         <v>-3.36</v>
       </c>
-      <c r="D17" s="1">
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="D18" s="2">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>89.17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="2">
         <v>0.6</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C19" s="2">
         <v>-3.43</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D19" s="2">
         <v>24.1</v>
       </c>
     </row>

</xml_diff>